<commit_message>
Rename quizzes to meaningful names; updates xls and remove unnecessary subjects
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/quiz_v1.xlsx
+++ b/app/src/main/res/raw/quiz_v1.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_quiz" sheetId="7" r:id="rId1"/>
-    <sheet name="quiz1" sheetId="1" r:id="rId2"/>
-    <sheet name="quiz2" sheetId="2" r:id="rId3"/>
-    <sheet name="quiz3" sheetId="3" r:id="rId4"/>
-    <sheet name="quiz4" sheetId="4" r:id="rId5"/>
-    <sheet name="quiz5" sheetId="5" r:id="rId6"/>
-    <sheet name="quiz6" sheetId="6" r:id="rId7"/>
+    <sheet name="quiz_geography1" sheetId="1" r:id="rId2"/>
+    <sheet name="quiz_politics1" sheetId="2" r:id="rId3"/>
+    <sheet name="quiz_environment1" sheetId="3" r:id="rId4"/>
+    <sheet name="quiz_independence1" sheetId="4" r:id="rId5"/>
+    <sheet name="quiz_environment2" sheetId="5" r:id="rId6"/>
+    <sheet name="quiz_politics2" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -1699,25 +1699,25 @@
     <t>Group2</t>
   </si>
   <si>
-    <t>quiz1</t>
-  </si>
-  <si>
-    <t>quiz2</t>
-  </si>
-  <si>
-    <t>quiz3</t>
-  </si>
-  <si>
-    <t>quiz4</t>
-  </si>
-  <si>
-    <t>quiz5</t>
-  </si>
-  <si>
-    <t>quiz6</t>
-  </si>
-  <si>
     <t>00_20_00</t>
+  </si>
+  <si>
+    <t>quiz_environment2</t>
+  </si>
+  <si>
+    <t>quiz_politics2</t>
+  </si>
+  <si>
+    <t>quiz_independence1</t>
+  </si>
+  <si>
+    <t>quiz_politics1</t>
+  </si>
+  <si>
+    <t>quiz_environment1</t>
+  </si>
+  <si>
+    <t>quiz_geography1</t>
   </si>
 </sst>
 </file>
@@ -2237,9 +2237,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2263,7 +2268,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -2278,12 +2283,12 @@
         <v>25</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="B3" t="s">
         <v>479</v>
@@ -2298,7 +2303,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
@@ -2312,13 +2317,13 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="B4" t="s">
         <v>479</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>260</v>
       </c>
       <c r="D4" t="s">
         <v>485</v>
@@ -2327,7 +2332,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
@@ -2356,7 +2361,7 @@
         <v>25</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
@@ -2370,7 +2375,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B6" t="s">
         <v>268</v>
@@ -2385,7 +2390,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
@@ -2399,7 +2404,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B7" t="s">
         <v>479</v>
@@ -2414,7 +2419,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
@@ -13275,13 +13280,16 @@
   </sheetPr>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58.83203125" customWidth="1"/>
+    <col min="12" max="12" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>